<commit_message>
made progress on grabbing excel data+ modified excel data to work with designed algo
</commit_message>
<xml_diff>
--- a/AnimalDiseaseQueryWebApp/Files/data.xlsx
+++ b/AnimalDiseaseQueryWebApp/Files/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spike\source\repos\AnimalDiseaseQueryPage\AnimalDiseaseQueryWebApp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89635785-690F-4342-AF2A-7180DCC31C49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59148496-52B8-4B64-BD9F-5A460B22FA6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11970" tabRatio="684" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11970" tabRatio="684" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disease-Sign Cattle" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Disease-Sign Camel" sheetId="8" r:id="rId5"/>
     <sheet name="Disease-Sign Horse_Mule" sheetId="9" r:id="rId6"/>
     <sheet name="Disease-Sign Donkey" sheetId="10" r:id="rId7"/>
+    <sheet name="Abbr" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="133">
-  <si>
-    <t>Constipation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="119">
   <si>
     <t>Diarrhoea</t>
   </si>
@@ -50,28 +48,16 @@
     <t>Ataixa / Incordination of movement</t>
   </si>
   <si>
-    <t>Dehydration</t>
-  </si>
-  <si>
     <t>Dysentery (Blood in faeces)</t>
   </si>
   <si>
     <t>Dyspnoea / Coughing (Difficulty breathing)</t>
   </si>
   <si>
-    <t>Icterus (Yellowing of membranes)</t>
-  </si>
-  <si>
     <t>Pyrexia / Fever</t>
   </si>
   <si>
     <t>Staring coat (Standing hair / rough coat)</t>
-  </si>
-  <si>
-    <t>Stunted growth or pot belly</t>
-  </si>
-  <si>
-    <t>Submandibular / Ventral oedema</t>
   </si>
   <si>
     <t>Weight loss / Emaciation (Loss of body condition)</t>
@@ -206,22 +192,6 @@
   </si>
   <si>
     <t>Anaemia / Pallor (Pale membranes)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Anorexia / (Loss of appetite)  / </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Depression</t>
-    </r>
   </si>
   <si>
     <r>
@@ -411,30 +381,6 @@
   </si>
   <si>
     <t>Swell</t>
-  </si>
-  <si>
-    <t>Abdominal pain / Rolling / Kicking stomach</t>
-  </si>
-  <si>
-    <t>Apathy / Depression</t>
-  </si>
-  <si>
-    <t>Breathing abnormal</t>
-  </si>
-  <si>
-    <t>Coughing (incl. owner reported)</t>
-  </si>
-  <si>
-    <t>Fecal output (Absense of)</t>
-  </si>
-  <si>
-    <t>Nasal discharge (mucopurulent)</t>
-  </si>
-  <si>
-    <t>Nasal discharge (serous)</t>
-  </si>
-  <si>
-    <t>Occular discharge / Involunatary closure of eyelid</t>
   </si>
   <si>
     <t>Abd_pain</t>
@@ -1187,7 +1133,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1197,57 +1145,57 @@
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="I1" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="J1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="K1" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="L1" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="M1" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="N1" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="P1" s="37" t="s">
         <v>62</v>
-      </c>
-      <c r="J1" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="P1" s="37" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" s="39">
         <v>2.5</v>
@@ -1299,7 +1247,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B3" s="39">
         <v>94.375</v>
@@ -1351,7 +1299,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" s="39">
         <v>5.625</v>
@@ -1403,7 +1351,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B5" s="39">
         <v>8.75</v>
@@ -1455,7 +1403,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B6" s="39">
         <v>11.875</v>
@@ -1507,7 +1455,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B7" s="39">
         <v>32.5</v>
@@ -1559,7 +1507,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B8" s="39">
         <v>79.375</v>
@@ -1611,7 +1559,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B9" s="41">
         <v>26.388888888888889</v>
@@ -1663,7 +1611,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B10" s="39">
         <v>18.611111111111111</v>
@@ -1715,7 +1663,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B11" s="41">
         <v>35.555555555555557</v>
@@ -1767,7 +1715,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B12" s="39">
         <v>5.625</v>
@@ -1819,7 +1767,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B13" s="39">
         <v>70.625</v>
@@ -1871,7 +1819,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B14" s="39">
         <v>2.5</v>
@@ -1923,7 +1871,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B15" s="39">
         <v>91.25</v>
@@ -1975,7 +1923,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B16" s="39">
         <v>20.625</v>
@@ -2027,7 +1975,7 @@
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B17" s="45">
         <v>79.375</v>
@@ -2114,132 +2062,68 @@
       <c r="P19" s="14"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="A21" s="9"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="7"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="7"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="A30" s="2"/>
+      <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="7"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="7"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="A33" s="10"/>
+      <c r="B33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="7"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="7"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2251,7 +2135,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFC37"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2262,66 +2148,66 @@
   <sheetData>
     <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="K1" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="L1" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="M1" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="47" t="s">
+      <c r="O1" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="P1" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="Q1" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="S1" s="48" t="s">
         <v>62</v>
-      </c>
-      <c r="L1" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="N1" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q1" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="R1" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="S1" s="48" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" s="49">
         <v>2.5</v>
@@ -2382,7 +2268,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" s="49">
         <v>2.5</v>
@@ -2443,7 +2329,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" s="49">
         <v>5.625</v>
@@ -2504,7 +2390,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B5" s="49">
         <v>64</v>
@@ -2565,7 +2451,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B6" s="49">
         <v>92.5</v>
@@ -2626,7 +2512,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B7" s="49">
         <v>2.5</v>
@@ -2687,7 +2573,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B8" s="49">
         <v>40.5</v>
@@ -2748,7 +2634,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B9" s="49">
         <v>5.625</v>
@@ -2809,7 +2695,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B10" s="49">
         <v>2.5</v>
@@ -2870,7 +2756,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B11" s="49">
         <v>7.5</v>
@@ -2931,7 +2817,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B12" s="49">
         <v>12</v>
@@ -2992,7 +2878,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B13" s="49">
         <v>12</v>
@@ -3053,7 +2939,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B14" s="49">
         <v>50</v>
@@ -3114,7 +3000,7 @@
     </row>
     <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="44" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B15" s="53">
         <v>92.5</v>
@@ -19581,192 +19467,116 @@
       <c r="XFC18" s="14"/>
     </row>
     <row r="19" spans="1:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="A19" s="9"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>55</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="18"/>
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>56</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="19"/>
       <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>57</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="20"/>
       <c r="D22" s="14"/>
     </row>
     <row r="23" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>58</v>
-      </c>
+      <c r="A23" s="24"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="19"/>
       <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>70</v>
-      </c>
+      <c r="A24" s="24"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="17"/>
       <c r="D24" s="14"/>
     </row>
     <row r="25" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>71</v>
-      </c>
+      <c r="A25" s="24"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="18"/>
       <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>59</v>
-      </c>
+      <c r="A26" s="24"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="18"/>
       <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>60</v>
-      </c>
+      <c r="A27" s="25"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="19"/>
       <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>61</v>
-      </c>
+      <c r="A28" s="25"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="19"/>
       <c r="D28" s="14"/>
     </row>
     <row r="29" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>62</v>
-      </c>
+      <c r="A29" s="25"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="19"/>
       <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>63</v>
-      </c>
+      <c r="A30" s="24"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="20"/>
       <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>72</v>
-      </c>
+      <c r="A31" s="24"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="17"/>
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:16383" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>64</v>
-      </c>
+      <c r="A32" s="24"/>
+      <c r="B32" s="21"/>
       <c r="C32" s="18"/>
       <c r="D32" s="14"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>65</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="21"/>
       <c r="C33" s="19"/>
       <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>66</v>
-      </c>
+      <c r="A34" s="22"/>
+      <c r="B34" s="21"/>
       <c r="C34" s="19"/>
       <c r="D34" s="14"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>69</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="21"/>
       <c r="C35" s="19"/>
       <c r="D35" s="14"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>67</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="21"/>
       <c r="C36" s="18"/>
       <c r="D36" s="14"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>68</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="19"/>
       <c r="D37" s="14"/>
     </row>
@@ -19783,7 +19593,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19793,66 +19605,66 @@
   <sheetData>
     <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="K1" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="L1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="M1" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="36" t="s">
+      <c r="O1" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="P1" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="Q1" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="S1" s="37" t="s">
         <v>62</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="N1" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q1" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="R1" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="S1" s="37" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B2" s="49">
         <v>5.625</v>
@@ -19913,7 +19725,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" s="49">
         <v>11.875</v>
@@ -19974,7 +19786,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B4" s="49">
         <v>2.5</v>
@@ -20035,7 +19847,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" s="49">
         <v>5.625</v>
@@ -20096,7 +19908,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" s="49">
         <v>2.5</v>
@@ -20157,7 +19969,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7" s="49">
         <v>17.5</v>
@@ -20218,7 +20030,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B8" s="49">
         <v>17.5</v>
@@ -20279,7 +20091,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B9" s="49">
         <v>2.5</v>
@@ -20340,7 +20152,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B10" s="49">
         <v>5.625</v>
@@ -20401,7 +20213,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B11" s="49">
         <v>17.5</v>
@@ -20462,7 +20274,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B12" s="49">
         <v>17.5</v>
@@ -20523,7 +20335,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B13" s="49">
         <v>32.5</v>
@@ -20584,7 +20396,7 @@
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="44" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B14" s="53">
         <v>91.25</v>
@@ -20691,194 +20503,118 @@
       <c r="A17"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="A18" s="9"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="U18" s="14"/>
       <c r="V18" s="3"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="13"/>
       <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="A21" s="25"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="16"/>
       <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="A22" s="24"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="15"/>
       <c r="D22" s="14"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>70</v>
-      </c>
+      <c r="A23" s="24"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="17"/>
       <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="A24" s="24"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="18"/>
       <c r="D24" s="14"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="A25" s="24"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="13"/>
       <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="A26" s="25"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="19"/>
       <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="A27" s="25"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="19"/>
       <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="A28" s="25"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="19"/>
       <c r="D28" s="14"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="A29" s="24"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="20"/>
       <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="A30" s="24"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="17"/>
       <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="A31" s="24"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="18"/>
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="A32" s="25"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="19"/>
       <c r="D32" s="14"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="A33" s="10"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="15"/>
       <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="15"/>
       <c r="D34" s="14"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="13"/>
       <c r="D35" s="14"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="7"/>
       <c r="C36" s="15"/>
       <c r="D36" s="14"/>
     </row>
@@ -20910,75 +20646,75 @@
   <sheetData>
     <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="N1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="R1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="S1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C2" s="14">
         <v>2.5</v>
@@ -21037,10 +20773,10 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C3" s="14">
         <v>2.5</v>
@@ -21099,10 +20835,10 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C4" s="14">
         <v>5.625</v>
@@ -21161,10 +20897,10 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C5" s="14">
         <v>5.625</v>
@@ -21223,10 +20959,10 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C6" s="14">
         <v>2.5</v>
@@ -21283,15 +21019,15 @@
         <v>2.5</v>
       </c>
       <c r="V6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" s="14">
         <v>2.5</v>
@@ -21348,15 +21084,15 @@
         <v>14.375</v>
       </c>
       <c r="V7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8" s="14">
         <v>17.5</v>
@@ -21415,10 +21151,10 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C9" s="14">
         <v>40.5</v>
@@ -21477,10 +21213,10 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C10" s="14">
         <v>17.5</v>
@@ -21539,10 +21275,10 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C11" s="14">
         <v>5.625</v>
@@ -21601,10 +21337,10 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="C12" s="14">
         <v>5.625</v>
@@ -21663,10 +21399,10 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C13" s="14">
         <v>7.5</v>
@@ -21725,10 +21461,10 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C14" s="14">
         <v>17.5</v>
@@ -21787,10 +21523,10 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C15" s="14">
         <v>12</v>
@@ -21849,10 +21585,10 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C16" s="14">
         <v>17.5</v>
@@ -21911,10 +21647,10 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C17" s="14">
         <v>12</v>
@@ -21973,10 +21709,10 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C18" s="14">
         <v>32.5</v>
@@ -22035,10 +21771,10 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C19" s="14">
         <v>50</v>
@@ -22119,66 +21855,66 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="L21" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="M21" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="N21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O21" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I21" s="5" t="s">
+      <c r="P21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="Q21" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="R21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="S21" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="T21" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="P21" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q21" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="R21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="S21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="T21" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C22" s="14">
         <f t="shared" ref="C22:T22" si="0">(C2-C3)/MIN(C2,C3)</f>
@@ -22253,20 +21989,20 @@
         <v>0.35714285714285715</v>
       </c>
       <c r="V22" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="V23" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C24" s="14">
         <f t="shared" ref="C24:T24" si="1">(C4-C5)/MIN(C4,C5)</f>
@@ -22341,20 +22077,20 @@
         <v>2.3571428571428572</v>
       </c>
       <c r="V24" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="V25" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C26" s="14">
         <f t="shared" ref="C26:T26" si="2">(C6-C7)/MIN(C6,C7)</f>
@@ -22431,12 +22167,12 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C28" s="14">
         <f t="shared" ref="C28:T28" si="3">(C8-C9)/MIN(C8,C9)</f>
@@ -22513,12 +22249,12 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C30" s="14">
         <f t="shared" ref="C30:T30" si="4">(C10-C11)/MIN(C10,C11)</f>
@@ -22595,12 +22331,12 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C32" s="14">
         <f t="shared" ref="C32:T32" si="5">(C12-C13)/MIN(C12,C13)</f>
@@ -22677,12 +22413,12 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C34" s="14">
         <f t="shared" ref="C34:T34" si="6">(C14-C15)/MIN(C14,C15)</f>
@@ -22759,12 +22495,12 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C36" s="14">
         <f t="shared" ref="C36:T36" si="7">(C16-C17)/MIN(C16,C17)</f>
@@ -22841,12 +22577,12 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C38" s="14">
         <f t="shared" ref="C38:T38" si="8">(C18-C19)/MIN(C18,C19)</f>
@@ -22923,7 +22659,7 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -22940,7 +22676,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22950,75 +22688,75 @@
   <sheetData>
     <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="T1" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="36" t="s">
+      <c r="U1" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="M1" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="O1" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="R1" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="S1" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="T1" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="U1" s="36" t="s">
-        <v>67</v>
-      </c>
       <c r="V1" s="37" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" s="49">
         <v>14.583333333333334</v>
@@ -23088,7 +22826,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B3" s="49">
         <v>93.333333333333329</v>
@@ -23158,7 +22896,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B4" s="56">
         <v>2.5</v>
@@ -23228,7 +22966,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B5" s="49">
         <v>4.583333333333333</v>
@@ -23298,7 +23036,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B6" s="49">
         <v>36.25</v>
@@ -23368,7 +23106,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B7" s="49">
         <v>5</v>
@@ -23438,7 +23176,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B8" s="49">
         <v>2.5</v>
@@ -23508,7 +23246,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B9" s="49">
         <v>5</v>
@@ -23578,7 +23316,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B10" s="49">
         <v>26.5</v>
@@ -23648,7 +23386,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B11" s="49">
         <v>47.5</v>
@@ -23718,7 +23456,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B12" s="49">
         <v>33.5</v>
@@ -23788,7 +23526,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B13" s="49">
         <v>2.5</v>
@@ -23858,7 +23596,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B14" s="49">
         <v>7.5</v>
@@ -23928,7 +23666,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B15" s="49">
         <v>24</v>
@@ -23998,7 +23736,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B16" s="49">
         <v>66.5</v>
@@ -24068,7 +23806,7 @@
     </row>
     <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B17" s="53">
         <v>85.416666666666671</v>
@@ -24188,219 +23926,131 @@
       <c r="A20"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="A21" s="9"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>93</v>
-      </c>
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="6"/>
       <c r="D22" s="14"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="6"/>
       <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="6"/>
       <c r="D24" s="14"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="A25" s="25"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="6"/>
       <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>94</v>
-      </c>
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="6"/>
       <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="A27" s="24"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="6"/>
       <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="A28" s="24"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="6"/>
       <c r="D28" s="14"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="A29" s="25"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="6"/>
       <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="A30" s="25"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>95</v>
-      </c>
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="6"/>
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>96</v>
-      </c>
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="A33" s="24"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="6"/>
       <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>97</v>
-      </c>
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="6"/>
       <c r="D34" s="14"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="A35" s="24"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="6"/>
       <c r="D35" s="14"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="A36" s="24"/>
+      <c r="B36" s="7"/>
       <c r="C36" s="6"/>
       <c r="D36" s="14"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="A37" s="25"/>
+      <c r="B37" s="7"/>
       <c r="C37" s="6"/>
       <c r="D37" s="14"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="A38" s="10"/>
+      <c r="B38" s="7"/>
       <c r="C38" s="6"/>
       <c r="D38" s="14"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>99</v>
-      </c>
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
       <c r="C39" s="6"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>100</v>
-      </c>
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
       <c r="C40" s="6"/>
       <c r="D40" s="14"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="A41" s="2"/>
+      <c r="B41" s="7"/>
       <c r="C41" s="6"/>
       <c r="D41" s="14"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="7"/>
       <c r="C42" s="6"/>
       <c r="D42" s="14"/>
     </row>
@@ -24538,7 +24188,7 @@
   <dimension ref="A1:V65"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:C45"/>
+      <selection activeCell="A25" sqref="A25:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24549,66 +24199,66 @@
   <sheetData>
     <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F1" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>63</v>
-      </c>
       <c r="M1" s="36" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="N1" s="36" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="O1" s="36" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="P1" s="36" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Q1" s="36" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="R1" s="36" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="S1" s="37" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B2" s="49">
         <v>14.375</v>
@@ -24669,7 +24319,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" s="49">
         <v>38.125</v>
@@ -24730,7 +24380,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B4" s="49">
         <v>67.5</v>
@@ -24791,7 +24441,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B5" s="49">
         <v>5.625</v>
@@ -24852,7 +24502,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B6" s="49">
         <v>91.25</v>
@@ -24913,7 +24563,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B7" s="49">
         <v>58.75</v>
@@ -24974,7 +24624,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B8" s="49">
         <v>5.625</v>
@@ -25035,7 +24685,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B9" s="49">
         <v>5.625</v>
@@ -25096,7 +24746,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B10" s="49">
         <v>2.5</v>
@@ -25157,7 +24807,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B11" s="49">
         <v>2.5</v>
@@ -25218,7 +24868,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B12" s="49">
         <v>2.5</v>
@@ -25279,7 +24929,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B13" s="49">
         <v>26.25</v>
@@ -25340,7 +24990,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="B14" s="56">
         <v>2.5</v>
@@ -25401,7 +25051,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B15" s="49">
         <v>2.5</v>
@@ -25462,7 +25112,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B16" s="49">
         <v>2.5</v>
@@ -25523,7 +25173,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B17" s="49">
         <v>2.5</v>
@@ -25584,7 +25234,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B18" s="56">
         <v>2.5</v>
@@ -25645,7 +25295,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B19" s="59">
         <v>5.625</v>
@@ -25706,7 +25356,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B20" s="49">
         <v>2.5</v>
@@ -25767,7 +25417,7 @@
     </row>
     <row r="21" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="44" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B21" s="53">
         <v>94.375</v>
@@ -25853,226 +25503,150 @@
       <c r="A24" s="55"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="A25" s="9"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="A26" s="31"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="31"/>
       <c r="D26" s="14"/>
       <c r="F26" s="31"/>
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="31"/>
       <c r="D27" s="14"/>
       <c r="F27" s="31"/>
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="31"/>
       <c r="D28" s="14"/>
       <c r="F28" s="31"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>110</v>
-      </c>
+      <c r="A29" s="31"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="31"/>
       <c r="D29" s="14"/>
       <c r="F29" s="31"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="A30" s="25"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="31"/>
       <c r="D30" s="14"/>
       <c r="F30" s="31"/>
       <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>111</v>
-      </c>
+      <c r="A31" s="31"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="31"/>
       <c r="D31" s="14"/>
       <c r="F31" s="31"/>
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>112</v>
-      </c>
+      <c r="A32" s="31"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="31"/>
       <c r="D32" s="14"/>
       <c r="F32" s="31"/>
       <c r="G32" s="14"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="A33" s="24"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="31"/>
       <c r="D33" s="14"/>
       <c r="F33" s="31"/>
       <c r="G33" s="14"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>113</v>
-      </c>
+      <c r="A34" s="31"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="31"/>
       <c r="D34" s="14"/>
       <c r="F34" s="31"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>95</v>
-      </c>
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="31"/>
       <c r="F35" s="31"/>
       <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="A36" s="24"/>
+      <c r="B36" s="7"/>
       <c r="C36" s="31"/>
       <c r="D36" s="14"/>
       <c r="F36" s="31"/>
       <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="A37" s="31"/>
+      <c r="B37" s="7"/>
       <c r="C37" s="31"/>
       <c r="D37" s="14"/>
       <c r="F37" s="31"/>
       <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>115</v>
-      </c>
+      <c r="A38" s="31"/>
+      <c r="B38" s="7"/>
       <c r="C38" s="31"/>
       <c r="D38" s="14"/>
       <c r="F38" s="31"/>
       <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="A39" s="24"/>
+      <c r="B39" s="7"/>
       <c r="C39" s="31"/>
       <c r="D39" s="14"/>
       <c r="F39" s="31"/>
       <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="A40" s="24"/>
+      <c r="B40" s="7"/>
       <c r="C40" s="31"/>
       <c r="D40" s="14"/>
       <c r="F40" s="31"/>
       <c r="G40" s="14"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>100</v>
-      </c>
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
       <c r="C41" s="31"/>
       <c r="D41" s="14"/>
       <c r="F41" s="31"/>
       <c r="G41" s="14"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="7"/>
       <c r="C42" s="31"/>
       <c r="D42" s="14"/>
       <c r="F42" s="31"/>
       <c r="G42" s="14"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="31"/>
       <c r="D43" s="14"/>
       <c r="F43" s="31"/>
@@ -26214,8 +25788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26226,66 +25800,66 @@
   <sheetData>
     <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F1" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>63</v>
-      </c>
       <c r="M1" s="36" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="N1" s="36" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="O1" s="36" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="P1" s="36" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Q1" s="36" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="R1" s="36" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="S1" s="37" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" s="49">
         <v>8.75</v>
@@ -26346,7 +25920,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B3" s="49">
         <v>67.5</v>
@@ -26407,7 +25981,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B4" s="49">
         <v>6.666666666666667</v>
@@ -26468,7 +26042,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B5" s="49">
         <v>61.875</v>
@@ -26529,7 +26103,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B6" s="49">
         <v>50</v>
@@ -26590,7 +26164,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B7" s="49">
         <v>5.625</v>
@@ -26651,7 +26225,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B8" s="49">
         <v>2.5</v>
@@ -26712,7 +26286,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B9" s="49">
         <v>2.5</v>
@@ -26773,7 +26347,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B10" s="49">
         <v>22.5</v>
@@ -26834,7 +26408,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="B11" s="56">
         <v>2.5</v>
@@ -26895,7 +26469,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B12" s="49">
         <v>2.5</v>
@@ -26956,7 +26530,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B13" s="49">
         <v>2.5</v>
@@ -27017,7 +26591,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B14" s="49">
         <v>2.5</v>
@@ -27078,7 +26652,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B15" s="56">
         <v>2.5</v>
@@ -27139,7 +26713,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B16" s="49">
         <v>5.625</v>
@@ -27200,7 +26774,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B17" s="49">
         <v>2.5</v>
@@ -27261,7 +26835,7 @@
     </row>
     <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="44" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B18" s="53">
         <v>95.9375</v>
@@ -27369,226 +26943,150 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="A22" s="9"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="A23" s="31"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="31"/>
       <c r="D23" s="14"/>
       <c r="F23" s="31"/>
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="31"/>
       <c r="D24" s="14"/>
       <c r="F24" s="31"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="31"/>
       <c r="D25" s="14"/>
       <c r="F25" s="31"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>110</v>
-      </c>
+      <c r="A26" s="31"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="31"/>
       <c r="D26" s="14"/>
       <c r="F26" s="31"/>
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="A27" s="25"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="31"/>
       <c r="D27" s="14"/>
       <c r="F27" s="31"/>
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>111</v>
-      </c>
+      <c r="A28" s="31"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="31"/>
       <c r="D28" s="14"/>
       <c r="F28" s="31"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>112</v>
-      </c>
+      <c r="A29" s="31"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="31"/>
       <c r="D29" s="14"/>
       <c r="F29" s="31"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="A30" s="24"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="31"/>
       <c r="D30" s="14"/>
       <c r="F30" s="31"/>
       <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>113</v>
-      </c>
+      <c r="A31" s="31"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="31"/>
       <c r="D31" s="14"/>
       <c r="F31" s="31"/>
     </row>
     <row r="32" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>95</v>
-      </c>
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="31"/>
       <c r="F32" s="31"/>
       <c r="G32" s="14"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="A33" s="24"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="31"/>
       <c r="D33" s="14"/>
       <c r="F33" s="31"/>
       <c r="G33" s="14"/>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="A34" s="31"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="31"/>
       <c r="D34" s="14"/>
       <c r="F34" s="31"/>
       <c r="G34" s="14"/>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>115</v>
-      </c>
+      <c r="A35" s="31"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="31"/>
       <c r="D35" s="14"/>
       <c r="F35" s="31"/>
       <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>132</v>
-      </c>
+      <c r="A36" s="24"/>
+      <c r="B36" s="7"/>
       <c r="C36" s="31"/>
       <c r="D36" s="14"/>
       <c r="F36" s="31"/>
       <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="A37" s="24"/>
+      <c r="B37" s="7"/>
       <c r="C37" s="31"/>
       <c r="D37" s="14"/>
       <c r="F37" s="31"/>
       <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>100</v>
-      </c>
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
       <c r="C38" s="31"/>
       <c r="D38" s="14"/>
       <c r="F38" s="31"/>
       <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="7"/>
       <c r="C39" s="31"/>
       <c r="D39" s="14"/>
       <c r="F39" s="31"/>
       <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="7"/>
       <c r="C40" s="31"/>
       <c r="D40" s="14"/>
       <c r="F40" s="31"/>
@@ -27724,4 +27222,195 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEAA06E-F330-4153-A681-769C8DA29C30}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
the excel file correctly loads, but disease probs need to be fixed as conversion defaults them to 0
</commit_message>
<xml_diff>
--- a/AnimalDiseaseQueryWebApp/Files/data.xlsx
+++ b/AnimalDiseaseQueryWebApp/Files/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spike\source\repos\AnimalDiseaseQueryPage\AnimalDiseaseQueryWebApp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59148496-52B8-4B64-BD9F-5A460B22FA6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50146A60-B657-49EC-82C2-647B08C21526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11970" tabRatio="684" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11970" tabRatio="684" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disease-Sign Cattle" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="133">
   <si>
     <t>Diarrhoea</t>
   </si>
@@ -453,6 +453,61 @@
   </si>
   <si>
     <t>Oc_Dis</t>
+  </si>
+  <si>
+    <t>Constipation</t>
+  </si>
+  <si>
+    <t>Dehydration</t>
+  </si>
+  <si>
+    <t>Icterus (Yellowing of membranes)</t>
+  </si>
+  <si>
+    <t>Stunted growth or pot belly</t>
+  </si>
+  <si>
+    <t>Submandibular / Ventral oedema</t>
+  </si>
+  <si>
+    <t>Abdominal pain / Rolling / Kicking stomach</t>
+  </si>
+  <si>
+    <t>Apathy / Depression</t>
+  </si>
+  <si>
+    <t>Breathing abnormal</t>
+  </si>
+  <si>
+    <t>Coughing (incl. owner reported)</t>
+  </si>
+  <si>
+    <t>Fecal output (Absense of)</t>
+  </si>
+  <si>
+    <t>Nasal discharge (mucopurulent)</t>
+  </si>
+  <si>
+    <t>Nasal discharge (serous)</t>
+  </si>
+  <si>
+    <t>Occular discharge / Involunatary closure of eyelid</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Anorexia / (Loss of appetite)  / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Depression</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -25788,7 +25843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:B40"/>
     </sheetView>
   </sheetViews>
@@ -27226,13 +27281,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEAA06E-F330-4153-A681-769C8DA29C30}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92:B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
@@ -27243,172 +27302,892 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>10</v>
+      <c r="A2" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B17" s="21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B18" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B19" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B57" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+    <row r="58" spans="1:2" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B61" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B63" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B64" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B65" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B66" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B67" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B68" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B69" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B70" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B72" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B73" s="7" t="s">
         <v>62</v>
       </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" s="56" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="56" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="31"/>
+      <c r="B110" s="7"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="24"/>
+      <c r="B111" s="7"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="24"/>
+      <c r="B112" s="7"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="6"/>
+      <c r="B113" s="7"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+      <c r="B114" s="7"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+      <c r="B115" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>